<commit_message>
best log and deleted useless files
</commit_message>
<xml_diff>
--- a/cifo_project_v2/cifo_project/log/mp0-8_0/run_21.xlsx
+++ b/cifo_project_v2/cifo_project/log/mp0-8_0/run_21.xlsx
@@ -391,7 +391,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="3">
@@ -402,7 +402,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="4">
@@ -413,7 +413,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="5">
@@ -424,7 +424,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="6">
@@ -435,7 +435,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="7">
@@ -446,7 +446,7 @@
         <v>5</v>
       </c>
       <c r="C7" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="8">
@@ -457,7 +457,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="9">
@@ -468,7 +468,7 @@
         <v>7</v>
       </c>
       <c r="C9" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="10">
@@ -479,7 +479,7 @@
         <v>8</v>
       </c>
       <c r="C10" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="11">
@@ -490,7 +490,7 @@
         <v>9</v>
       </c>
       <c r="C11" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="12">
@@ -501,7 +501,7 @@
         <v>10</v>
       </c>
       <c r="C12" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="13">
@@ -512,7 +512,7 @@
         <v>11</v>
       </c>
       <c r="C13" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="14">
@@ -523,7 +523,7 @@
         <v>12</v>
       </c>
       <c r="C14" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="15">
@@ -534,7 +534,7 @@
         <v>13</v>
       </c>
       <c r="C15" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="16">
@@ -545,7 +545,7 @@
         <v>14</v>
       </c>
       <c r="C16" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="17">
@@ -556,7 +556,7 @@
         <v>15</v>
       </c>
       <c r="C17" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="18">
@@ -567,7 +567,7 @@
         <v>16</v>
       </c>
       <c r="C18" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="19">
@@ -578,7 +578,7 @@
         <v>17</v>
       </c>
       <c r="C19" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="20">
@@ -589,7 +589,7 @@
         <v>18</v>
       </c>
       <c r="C20" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="21">
@@ -600,7 +600,7 @@
         <v>19</v>
       </c>
       <c r="C21" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="22">
@@ -611,7 +611,7 @@
         <v>20</v>
       </c>
       <c r="C22" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="23">
@@ -622,7 +622,7 @@
         <v>21</v>
       </c>
       <c r="C23" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="24">
@@ -633,7 +633,7 @@
         <v>22</v>
       </c>
       <c r="C24" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="25">
@@ -644,7 +644,7 @@
         <v>23</v>
       </c>
       <c r="C25" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="26">
@@ -655,7 +655,7 @@
         <v>24</v>
       </c>
       <c r="C26" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="27">
@@ -666,7 +666,7 @@
         <v>25</v>
       </c>
       <c r="C27" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="28">
@@ -677,7 +677,7 @@
         <v>26</v>
       </c>
       <c r="C28" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="29">
@@ -688,7 +688,7 @@
         <v>27</v>
       </c>
       <c r="C29" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="30">
@@ -699,7 +699,7 @@
         <v>28</v>
       </c>
       <c r="C30" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="31">
@@ -710,7 +710,7 @@
         <v>29</v>
       </c>
       <c r="C31" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="32">
@@ -721,7 +721,7 @@
         <v>30</v>
       </c>
       <c r="C32" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="33">
@@ -732,7 +732,7 @@
         <v>31</v>
       </c>
       <c r="C33" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="34">
@@ -743,7 +743,7 @@
         <v>32</v>
       </c>
       <c r="C34" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="35">
@@ -754,7 +754,7 @@
         <v>33</v>
       </c>
       <c r="C35" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="36">
@@ -765,7 +765,7 @@
         <v>34</v>
       </c>
       <c r="C36" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="37">
@@ -776,7 +776,7 @@
         <v>35</v>
       </c>
       <c r="C37" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="38">
@@ -787,7 +787,7 @@
         <v>36</v>
       </c>
       <c r="C38" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="39">
@@ -798,7 +798,7 @@
         <v>37</v>
       </c>
       <c r="C39" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="40">
@@ -809,7 +809,7 @@
         <v>38</v>
       </c>
       <c r="C40" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="41">
@@ -820,7 +820,7 @@
         <v>39</v>
       </c>
       <c r="C41" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="42">
@@ -831,7 +831,7 @@
         <v>40</v>
       </c>
       <c r="C42" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="43">
@@ -842,7 +842,7 @@
         <v>41</v>
       </c>
       <c r="C43" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="44">
@@ -853,7 +853,7 @@
         <v>42</v>
       </c>
       <c r="C44" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="45">
@@ -864,7 +864,7 @@
         <v>43</v>
       </c>
       <c r="C45" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="46">
@@ -875,7 +875,7 @@
         <v>44</v>
       </c>
       <c r="C46" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="47">
@@ -886,7 +886,7 @@
         <v>45</v>
       </c>
       <c r="C47" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="48">
@@ -897,7 +897,7 @@
         <v>46</v>
       </c>
       <c r="C48" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="49">
@@ -908,7 +908,7 @@
         <v>47</v>
       </c>
       <c r="C49" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="50">
@@ -919,7 +919,7 @@
         <v>48</v>
       </c>
       <c r="C50" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="51">
@@ -930,7 +930,7 @@
         <v>49</v>
       </c>
       <c r="C51" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="52">
@@ -941,7 +941,7 @@
         <v>50</v>
       </c>
       <c r="C52" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="53">
@@ -952,7 +952,7 @@
         <v>51</v>
       </c>
       <c r="C53" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="54">
@@ -963,7 +963,7 @@
         <v>52</v>
       </c>
       <c r="C54" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="55">
@@ -974,7 +974,7 @@
         <v>53</v>
       </c>
       <c r="C55" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="56">
@@ -985,7 +985,7 @@
         <v>54</v>
       </c>
       <c r="C56" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="57">
@@ -996,7 +996,7 @@
         <v>55</v>
       </c>
       <c r="C57" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="58">
@@ -1007,7 +1007,7 @@
         <v>56</v>
       </c>
       <c r="C58" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="59">
@@ -1018,7 +1018,7 @@
         <v>57</v>
       </c>
       <c r="C59" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="60">
@@ -1029,7 +1029,7 @@
         <v>58</v>
       </c>
       <c r="C60" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="61">
@@ -1040,7 +1040,7 @@
         <v>59</v>
       </c>
       <c r="C61" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="62">
@@ -1051,7 +1051,7 @@
         <v>60</v>
       </c>
       <c r="C62" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="63">
@@ -1062,7 +1062,7 @@
         <v>61</v>
       </c>
       <c r="C63" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="64">
@@ -1073,7 +1073,7 @@
         <v>62</v>
       </c>
       <c r="C64" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="65">
@@ -1084,7 +1084,7 @@
         <v>63</v>
       </c>
       <c r="C65" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="66">
@@ -1095,7 +1095,7 @@
         <v>64</v>
       </c>
       <c r="C66" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="67">
@@ -1106,7 +1106,7 @@
         <v>65</v>
       </c>
       <c r="C67" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="68">
@@ -1117,7 +1117,7 @@
         <v>66</v>
       </c>
       <c r="C68" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="69">
@@ -1128,7 +1128,7 @@
         <v>67</v>
       </c>
       <c r="C69" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="70">
@@ -1139,7 +1139,7 @@
         <v>68</v>
       </c>
       <c r="C70" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="71">
@@ -1150,7 +1150,7 @@
         <v>69</v>
       </c>
       <c r="C71" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="72">
@@ -1161,7 +1161,7 @@
         <v>70</v>
       </c>
       <c r="C72" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="73">
@@ -1172,7 +1172,7 @@
         <v>71</v>
       </c>
       <c r="C73" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="74">
@@ -1183,7 +1183,7 @@
         <v>72</v>
       </c>
       <c r="C74" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="75">
@@ -1194,7 +1194,7 @@
         <v>73</v>
       </c>
       <c r="C75" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="76">
@@ -1205,7 +1205,7 @@
         <v>74</v>
       </c>
       <c r="C76" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="77">
@@ -1216,7 +1216,7 @@
         <v>75</v>
       </c>
       <c r="C77" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="78">
@@ -1227,7 +1227,7 @@
         <v>76</v>
       </c>
       <c r="C78" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="79">
@@ -1238,7 +1238,7 @@
         <v>77</v>
       </c>
       <c r="C79" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="80">
@@ -1249,7 +1249,7 @@
         <v>78</v>
       </c>
       <c r="C80" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="81">
@@ -1260,7 +1260,7 @@
         <v>79</v>
       </c>
       <c r="C81" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="82">
@@ -1271,7 +1271,7 @@
         <v>80</v>
       </c>
       <c r="C82" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="83">
@@ -1282,7 +1282,7 @@
         <v>81</v>
       </c>
       <c r="C83" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="84">
@@ -1293,7 +1293,7 @@
         <v>82</v>
       </c>
       <c r="C84" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="85">
@@ -1304,7 +1304,7 @@
         <v>83</v>
       </c>
       <c r="C85" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="86">
@@ -1315,7 +1315,7 @@
         <v>84</v>
       </c>
       <c r="C86" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="87">
@@ -1326,7 +1326,7 @@
         <v>85</v>
       </c>
       <c r="C87" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="88">
@@ -1337,7 +1337,7 @@
         <v>86</v>
       </c>
       <c r="C88" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="89">
@@ -1348,7 +1348,7 @@
         <v>87</v>
       </c>
       <c r="C89" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="90">
@@ -1359,7 +1359,7 @@
         <v>88</v>
       </c>
       <c r="C90" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="91">
@@ -1370,7 +1370,7 @@
         <v>89</v>
       </c>
       <c r="C91" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="92">
@@ -1381,7 +1381,7 @@
         <v>90</v>
       </c>
       <c r="C92" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="93">
@@ -1392,7 +1392,7 @@
         <v>91</v>
       </c>
       <c r="C93" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="94">
@@ -1403,7 +1403,7 @@
         <v>92</v>
       </c>
       <c r="C94" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="95">
@@ -1414,7 +1414,7 @@
         <v>93</v>
       </c>
       <c r="C95" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="96">
@@ -1425,7 +1425,7 @@
         <v>94</v>
       </c>
       <c r="C96" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="97">
@@ -1436,7 +1436,7 @@
         <v>95</v>
       </c>
       <c r="C97" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="98">
@@ -1447,7 +1447,7 @@
         <v>96</v>
       </c>
       <c r="C98" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="99">
@@ -1458,7 +1458,7 @@
         <v>97</v>
       </c>
       <c r="C99" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="100">
@@ -1469,7 +1469,7 @@
         <v>98</v>
       </c>
       <c r="C100" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="101">
@@ -1480,7 +1480,7 @@
         <v>99</v>
       </c>
       <c r="C101" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="102">
@@ -1491,7 +1491,7 @@
         <v>100</v>
       </c>
       <c r="C102" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="103">
@@ -1502,7 +1502,7 @@
         <v>101</v>
       </c>
       <c r="C103" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="104">
@@ -1513,7 +1513,7 @@
         <v>102</v>
       </c>
       <c r="C104" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="105">
@@ -1524,7 +1524,7 @@
         <v>103</v>
       </c>
       <c r="C105" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="106">
@@ -1535,7 +1535,7 @@
         <v>104</v>
       </c>
       <c r="C106" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="107">
@@ -1546,7 +1546,7 @@
         <v>105</v>
       </c>
       <c r="C107" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="108">
@@ -1557,7 +1557,7 @@
         <v>106</v>
       </c>
       <c r="C108" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="109">
@@ -1568,7 +1568,7 @@
         <v>107</v>
       </c>
       <c r="C109" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="110">
@@ -1579,7 +1579,7 @@
         <v>108</v>
       </c>
       <c r="C110" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="111">
@@ -1590,7 +1590,7 @@
         <v>109</v>
       </c>
       <c r="C111" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="112">
@@ -1601,7 +1601,7 @@
         <v>110</v>
       </c>
       <c r="C112" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="113">
@@ -1612,7 +1612,7 @@
         <v>111</v>
       </c>
       <c r="C113" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="114">
@@ -1623,7 +1623,7 @@
         <v>112</v>
       </c>
       <c r="C114" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="115">
@@ -1634,7 +1634,7 @@
         <v>113</v>
       </c>
       <c r="C115" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="116">
@@ -1645,7 +1645,7 @@
         <v>114</v>
       </c>
       <c r="C116" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="117">
@@ -1656,7 +1656,7 @@
         <v>115</v>
       </c>
       <c r="C117" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="118">
@@ -1667,7 +1667,7 @@
         <v>116</v>
       </c>
       <c r="C118" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="119">
@@ -1678,7 +1678,7 @@
         <v>117</v>
       </c>
       <c r="C119" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="120">
@@ -1689,7 +1689,7 @@
         <v>118</v>
       </c>
       <c r="C120" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="121">
@@ -1700,7 +1700,7 @@
         <v>119</v>
       </c>
       <c r="C121" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="122">
@@ -1711,7 +1711,7 @@
         <v>120</v>
       </c>
       <c r="C122" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="123">
@@ -1722,7 +1722,7 @@
         <v>121</v>
       </c>
       <c r="C123" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="124">
@@ -1733,7 +1733,7 @@
         <v>122</v>
       </c>
       <c r="C124" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="125">
@@ -1744,7 +1744,7 @@
         <v>123</v>
       </c>
       <c r="C125" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="126">
@@ -1755,7 +1755,7 @@
         <v>124</v>
       </c>
       <c r="C126" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="127">
@@ -1766,7 +1766,7 @@
         <v>125</v>
       </c>
       <c r="C127" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="128">
@@ -1777,7 +1777,7 @@
         <v>126</v>
       </c>
       <c r="C128" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="129">
@@ -1788,7 +1788,7 @@
         <v>127</v>
       </c>
       <c r="C129" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="130">
@@ -1799,7 +1799,7 @@
         <v>128</v>
       </c>
       <c r="C130" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="131">
@@ -1810,7 +1810,7 @@
         <v>129</v>
       </c>
       <c r="C131" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="132">
@@ -1821,7 +1821,7 @@
         <v>130</v>
       </c>
       <c r="C132" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="133">
@@ -1832,7 +1832,7 @@
         <v>131</v>
       </c>
       <c r="C133" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="134">
@@ -1843,7 +1843,7 @@
         <v>132</v>
       </c>
       <c r="C134" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="135">
@@ -1854,7 +1854,7 @@
         <v>133</v>
       </c>
       <c r="C135" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="136">
@@ -1865,7 +1865,7 @@
         <v>134</v>
       </c>
       <c r="C136" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="137">
@@ -1876,7 +1876,7 @@
         <v>135</v>
       </c>
       <c r="C137" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="138">
@@ -1887,7 +1887,7 @@
         <v>136</v>
       </c>
       <c r="C138" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="139">
@@ -1898,7 +1898,7 @@
         <v>137</v>
       </c>
       <c r="C139" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="140">
@@ -1909,7 +1909,7 @@
         <v>138</v>
       </c>
       <c r="C140" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="141">
@@ -1920,7 +1920,7 @@
         <v>139</v>
       </c>
       <c r="C141" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="142">
@@ -1931,7 +1931,7 @@
         <v>140</v>
       </c>
       <c r="C142" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="143">
@@ -1942,7 +1942,7 @@
         <v>141</v>
       </c>
       <c r="C143" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="144">
@@ -1953,7 +1953,7 @@
         <v>142</v>
       </c>
       <c r="C144" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="145">
@@ -1964,7 +1964,7 @@
         <v>143</v>
       </c>
       <c r="C145" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="146">
@@ -1975,7 +1975,7 @@
         <v>144</v>
       </c>
       <c r="C146" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="147">
@@ -1986,7 +1986,7 @@
         <v>145</v>
       </c>
       <c r="C147" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="148">
@@ -1997,7 +1997,7 @@
         <v>146</v>
       </c>
       <c r="C148" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="149">
@@ -2008,7 +2008,7 @@
         <v>147</v>
       </c>
       <c r="C149" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="150">
@@ -2019,7 +2019,7 @@
         <v>148</v>
       </c>
       <c r="C150" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="151">
@@ -2030,7 +2030,7 @@
         <v>149</v>
       </c>
       <c r="C151" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="152">
@@ -2041,7 +2041,7 @@
         <v>150</v>
       </c>
       <c r="C152" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="153">
@@ -2052,7 +2052,7 @@
         <v>151</v>
       </c>
       <c r="C153" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="154">
@@ -2063,7 +2063,7 @@
         <v>152</v>
       </c>
       <c r="C154" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="155">
@@ -2074,7 +2074,7 @@
         <v>153</v>
       </c>
       <c r="C155" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="156">
@@ -2085,7 +2085,7 @@
         <v>154</v>
       </c>
       <c r="C156" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="157">
@@ -2096,7 +2096,7 @@
         <v>155</v>
       </c>
       <c r="C157" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="158">
@@ -2107,7 +2107,7 @@
         <v>156</v>
       </c>
       <c r="C158" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="159">
@@ -2118,7 +2118,7 @@
         <v>157</v>
       </c>
       <c r="C159" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="160">
@@ -2129,7 +2129,7 @@
         <v>158</v>
       </c>
       <c r="C160" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="161">
@@ -2140,7 +2140,7 @@
         <v>159</v>
       </c>
       <c r="C161" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="162">
@@ -2151,7 +2151,7 @@
         <v>160</v>
       </c>
       <c r="C162" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="163">
@@ -2162,7 +2162,7 @@
         <v>161</v>
       </c>
       <c r="C163" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="164">
@@ -2173,7 +2173,7 @@
         <v>162</v>
       </c>
       <c r="C164" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="165">
@@ -2184,7 +2184,7 @@
         <v>163</v>
       </c>
       <c r="C165" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="166">
@@ -2195,7 +2195,7 @@
         <v>164</v>
       </c>
       <c r="C166" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="167">
@@ -2206,7 +2206,7 @@
         <v>165</v>
       </c>
       <c r="C167" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="168">
@@ -2217,7 +2217,7 @@
         <v>166</v>
       </c>
       <c r="C168" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="169">
@@ -2228,7 +2228,7 @@
         <v>167</v>
       </c>
       <c r="C169" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="170">
@@ -2239,7 +2239,7 @@
         <v>168</v>
       </c>
       <c r="C170" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="171">
@@ -2250,7 +2250,7 @@
         <v>169</v>
       </c>
       <c r="C171" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="172">
@@ -2261,7 +2261,7 @@
         <v>170</v>
       </c>
       <c r="C172" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="173">
@@ -2272,7 +2272,7 @@
         <v>171</v>
       </c>
       <c r="C173" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="174">
@@ -2283,7 +2283,7 @@
         <v>172</v>
       </c>
       <c r="C174" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="175">
@@ -2294,7 +2294,7 @@
         <v>173</v>
       </c>
       <c r="C175" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="176">
@@ -2305,7 +2305,7 @@
         <v>174</v>
       </c>
       <c r="C176" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="177">
@@ -2316,7 +2316,7 @@
         <v>175</v>
       </c>
       <c r="C177" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="178">
@@ -2327,7 +2327,7 @@
         <v>176</v>
       </c>
       <c r="C178" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="179">
@@ -2338,7 +2338,7 @@
         <v>177</v>
       </c>
       <c r="C179" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="180">
@@ -2349,7 +2349,7 @@
         <v>178</v>
       </c>
       <c r="C180" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="181">
@@ -2360,7 +2360,7 @@
         <v>179</v>
       </c>
       <c r="C181" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="182">
@@ -2371,7 +2371,7 @@
         <v>180</v>
       </c>
       <c r="C182" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="183">
@@ -2382,7 +2382,7 @@
         <v>181</v>
       </c>
       <c r="C183" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="184">
@@ -2393,7 +2393,7 @@
         <v>182</v>
       </c>
       <c r="C184" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="185">
@@ -2404,7 +2404,7 @@
         <v>183</v>
       </c>
       <c r="C185" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="186">
@@ -2415,7 +2415,7 @@
         <v>184</v>
       </c>
       <c r="C186" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="187">
@@ -2426,7 +2426,7 @@
         <v>185</v>
       </c>
       <c r="C187" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="188">
@@ -2437,7 +2437,7 @@
         <v>186</v>
       </c>
       <c r="C188" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="189">
@@ -2448,7 +2448,7 @@
         <v>187</v>
       </c>
       <c r="C189" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="190">
@@ -2459,7 +2459,7 @@
         <v>188</v>
       </c>
       <c r="C190" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="191">
@@ -2470,7 +2470,7 @@
         <v>189</v>
       </c>
       <c r="C191" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="192">
@@ -2481,7 +2481,7 @@
         <v>190</v>
       </c>
       <c r="C192" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="193">
@@ -2492,7 +2492,7 @@
         <v>191</v>
       </c>
       <c r="C193" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="194">
@@ -2503,7 +2503,7 @@
         <v>192</v>
       </c>
       <c r="C194" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="195">
@@ -2514,7 +2514,7 @@
         <v>193</v>
       </c>
       <c r="C195" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="196">
@@ -2525,7 +2525,7 @@
         <v>194</v>
       </c>
       <c r="C196" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="197">
@@ -2536,7 +2536,7 @@
         <v>195</v>
       </c>
       <c r="C197" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="198">
@@ -2547,7 +2547,7 @@
         <v>196</v>
       </c>
       <c r="C198" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="199">
@@ -2558,7 +2558,7 @@
         <v>197</v>
       </c>
       <c r="C199" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="200">
@@ -2569,7 +2569,7 @@
         <v>198</v>
       </c>
       <c r="C200" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="201">
@@ -2580,7 +2580,7 @@
         <v>199</v>
       </c>
       <c r="C201" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="202">
@@ -2591,7 +2591,7 @@
         <v>200</v>
       </c>
       <c r="C202" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="203">
@@ -2602,7 +2602,7 @@
         <v>201</v>
       </c>
       <c r="C203" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="204">
@@ -2613,7 +2613,7 @@
         <v>202</v>
       </c>
       <c r="C204" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="205">
@@ -2624,7 +2624,7 @@
         <v>203</v>
       </c>
       <c r="C205" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="206">
@@ -2635,7 +2635,7 @@
         <v>204</v>
       </c>
       <c r="C206" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="207">
@@ -2646,7 +2646,7 @@
         <v>205</v>
       </c>
       <c r="C207" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="208">
@@ -2657,7 +2657,7 @@
         <v>206</v>
       </c>
       <c r="C208" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="209">
@@ -2668,7 +2668,7 @@
         <v>207</v>
       </c>
       <c r="C209" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="210">
@@ -2679,7 +2679,7 @@
         <v>208</v>
       </c>
       <c r="C210" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="211">
@@ -2690,7 +2690,7 @@
         <v>209</v>
       </c>
       <c r="C211" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="212">
@@ -2701,7 +2701,7 @@
         <v>210</v>
       </c>
       <c r="C212" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="213">
@@ -2712,7 +2712,7 @@
         <v>211</v>
       </c>
       <c r="C213" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="214">
@@ -2723,7 +2723,7 @@
         <v>212</v>
       </c>
       <c r="C214" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="215">
@@ -2734,7 +2734,7 @@
         <v>213</v>
       </c>
       <c r="C215" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="216">
@@ -2745,7 +2745,7 @@
         <v>214</v>
       </c>
       <c r="C216" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="217">
@@ -2756,7 +2756,7 @@
         <v>215</v>
       </c>
       <c r="C217" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="218">
@@ -2767,7 +2767,7 @@
         <v>216</v>
       </c>
       <c r="C218" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="219">
@@ -2778,7 +2778,7 @@
         <v>217</v>
       </c>
       <c r="C219" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="220">
@@ -2789,7 +2789,7 @@
         <v>218</v>
       </c>
       <c r="C220" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="221">
@@ -2800,7 +2800,7 @@
         <v>219</v>
       </c>
       <c r="C221" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="222">
@@ -2811,7 +2811,7 @@
         <v>220</v>
       </c>
       <c r="C222" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="223">
@@ -2822,7 +2822,7 @@
         <v>221</v>
       </c>
       <c r="C223" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="224">
@@ -2833,7 +2833,7 @@
         <v>222</v>
       </c>
       <c r="C224" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="225">
@@ -2844,7 +2844,7 @@
         <v>223</v>
       </c>
       <c r="C225" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="226">
@@ -2855,7 +2855,7 @@
         <v>224</v>
       </c>
       <c r="C226" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="227">
@@ -2866,7 +2866,7 @@
         <v>225</v>
       </c>
       <c r="C227" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="228">
@@ -2877,7 +2877,7 @@
         <v>226</v>
       </c>
       <c r="C228" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="229">
@@ -2888,7 +2888,7 @@
         <v>227</v>
       </c>
       <c r="C229" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="230">
@@ -2899,7 +2899,7 @@
         <v>228</v>
       </c>
       <c r="C230" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="231">
@@ -2910,7 +2910,7 @@
         <v>229</v>
       </c>
       <c r="C231" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="232">
@@ -2921,7 +2921,7 @@
         <v>230</v>
       </c>
       <c r="C232" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="233">
@@ -2932,7 +2932,7 @@
         <v>231</v>
       </c>
       <c r="C233" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="234">
@@ -2943,7 +2943,7 @@
         <v>232</v>
       </c>
       <c r="C234" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="235">
@@ -2954,7 +2954,7 @@
         <v>233</v>
       </c>
       <c r="C235" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="236">
@@ -2965,7 +2965,7 @@
         <v>234</v>
       </c>
       <c r="C236" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="237">
@@ -2976,7 +2976,7 @@
         <v>235</v>
       </c>
       <c r="C237" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="238">
@@ -2987,7 +2987,7 @@
         <v>236</v>
       </c>
       <c r="C238" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="239">
@@ -2998,7 +2998,7 @@
         <v>237</v>
       </c>
       <c r="C239" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="240">
@@ -3009,7 +3009,7 @@
         <v>238</v>
       </c>
       <c r="C240" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="241">
@@ -3020,7 +3020,7 @@
         <v>239</v>
       </c>
       <c r="C241" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="242">
@@ -3031,7 +3031,7 @@
         <v>240</v>
       </c>
       <c r="C242" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="243">
@@ -3042,7 +3042,7 @@
         <v>241</v>
       </c>
       <c r="C243" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="244">
@@ -3053,7 +3053,7 @@
         <v>242</v>
       </c>
       <c r="C244" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="245">
@@ -3064,7 +3064,7 @@
         <v>243</v>
       </c>
       <c r="C245" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="246">
@@ -3075,7 +3075,7 @@
         <v>244</v>
       </c>
       <c r="C246" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="247">
@@ -3086,7 +3086,7 @@
         <v>245</v>
       </c>
       <c r="C247" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="248">
@@ -3097,7 +3097,7 @@
         <v>246</v>
       </c>
       <c r="C248" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="249">
@@ -3108,7 +3108,7 @@
         <v>247</v>
       </c>
       <c r="C249" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="250">
@@ -3119,7 +3119,7 @@
         <v>248</v>
       </c>
       <c r="C250" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="251">
@@ -3130,7 +3130,7 @@
         <v>249</v>
       </c>
       <c r="C251" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="252">
@@ -3141,7 +3141,7 @@
         <v>250</v>
       </c>
       <c r="C252" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="253">
@@ -3152,7 +3152,7 @@
         <v>251</v>
       </c>
       <c r="C253" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="254">
@@ -3163,7 +3163,7 @@
         <v>252</v>
       </c>
       <c r="C254" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="255">
@@ -3174,7 +3174,7 @@
         <v>253</v>
       </c>
       <c r="C255" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="256">
@@ -3185,7 +3185,7 @@
         <v>254</v>
       </c>
       <c r="C256" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="257">
@@ -3196,7 +3196,7 @@
         <v>255</v>
       </c>
       <c r="C257" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="258">
@@ -3207,7 +3207,7 @@
         <v>256</v>
       </c>
       <c r="C258" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="259">
@@ -3218,7 +3218,7 @@
         <v>257</v>
       </c>
       <c r="C259" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="260">
@@ -3229,7 +3229,7 @@
         <v>258</v>
       </c>
       <c r="C260" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="261">
@@ -3240,7 +3240,7 @@
         <v>259</v>
       </c>
       <c r="C261" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="262">
@@ -3251,7 +3251,7 @@
         <v>260</v>
       </c>
       <c r="C262" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="263">
@@ -3262,7 +3262,7 @@
         <v>261</v>
       </c>
       <c r="C263" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="264">
@@ -3273,7 +3273,7 @@
         <v>262</v>
       </c>
       <c r="C264" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="265">
@@ -3284,7 +3284,7 @@
         <v>263</v>
       </c>
       <c r="C265" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="266">
@@ -3295,7 +3295,7 @@
         <v>264</v>
       </c>
       <c r="C266" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="267">
@@ -3306,7 +3306,7 @@
         <v>265</v>
       </c>
       <c r="C267" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="268">
@@ -3317,7 +3317,7 @@
         <v>266</v>
       </c>
       <c r="C268" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="269">
@@ -3328,7 +3328,7 @@
         <v>267</v>
       </c>
       <c r="C269" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="270">
@@ -3339,7 +3339,7 @@
         <v>268</v>
       </c>
       <c r="C270" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="271">
@@ -3350,7 +3350,7 @@
         <v>269</v>
       </c>
       <c r="C271" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="272">
@@ -3361,7 +3361,7 @@
         <v>270</v>
       </c>
       <c r="C272" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="273">
@@ -3372,7 +3372,7 @@
         <v>271</v>
       </c>
       <c r="C273" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="274">
@@ -3383,7 +3383,7 @@
         <v>272</v>
       </c>
       <c r="C274" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="275">
@@ -3394,7 +3394,7 @@
         <v>273</v>
       </c>
       <c r="C275" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="276">
@@ -3405,7 +3405,7 @@
         <v>274</v>
       </c>
       <c r="C276" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="277">
@@ -3416,7 +3416,7 @@
         <v>275</v>
       </c>
       <c r="C277" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="278">
@@ -3427,7 +3427,7 @@
         <v>276</v>
       </c>
       <c r="C278" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="279">
@@ -3438,7 +3438,7 @@
         <v>277</v>
       </c>
       <c r="C279" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="280">
@@ -3449,7 +3449,7 @@
         <v>278</v>
       </c>
       <c r="C280" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="281">
@@ -3460,7 +3460,7 @@
         <v>279</v>
       </c>
       <c r="C281" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="282">
@@ -3471,7 +3471,7 @@
         <v>280</v>
       </c>
       <c r="C282" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="283">
@@ -3482,7 +3482,7 @@
         <v>281</v>
       </c>
       <c r="C283" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="284">
@@ -3493,7 +3493,7 @@
         <v>282</v>
       </c>
       <c r="C284" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="285">
@@ -3504,7 +3504,7 @@
         <v>283</v>
       </c>
       <c r="C285" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="286">
@@ -3515,7 +3515,7 @@
         <v>284</v>
       </c>
       <c r="C286" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="287">
@@ -3526,7 +3526,7 @@
         <v>285</v>
       </c>
       <c r="C287" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="288">
@@ -3537,7 +3537,7 @@
         <v>286</v>
       </c>
       <c r="C288" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="289">
@@ -3548,7 +3548,7 @@
         <v>287</v>
       </c>
       <c r="C289" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="290">
@@ -3559,7 +3559,7 @@
         <v>288</v>
       </c>
       <c r="C290" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="291">
@@ -3570,7 +3570,7 @@
         <v>289</v>
       </c>
       <c r="C291" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="292">
@@ -3581,7 +3581,7 @@
         <v>290</v>
       </c>
       <c r="C292" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="293">
@@ -3592,7 +3592,7 @@
         <v>291</v>
       </c>
       <c r="C293" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="294">
@@ -3603,7 +3603,7 @@
         <v>292</v>
       </c>
       <c r="C294" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="295">
@@ -3614,7 +3614,7 @@
         <v>293</v>
       </c>
       <c r="C295" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="296">
@@ -3625,7 +3625,7 @@
         <v>294</v>
       </c>
       <c r="C296" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="297">
@@ -3636,7 +3636,7 @@
         <v>295</v>
       </c>
       <c r="C297" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="298">
@@ -3647,7 +3647,7 @@
         <v>296</v>
       </c>
       <c r="C298" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="299">
@@ -3658,7 +3658,7 @@
         <v>297</v>
       </c>
       <c r="C299" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="300">
@@ -3669,7 +3669,7 @@
         <v>298</v>
       </c>
       <c r="C300" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="301">
@@ -3680,7 +3680,7 @@
         <v>299</v>
       </c>
       <c r="C301" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="302">
@@ -3691,7 +3691,7 @@
         <v>300</v>
       </c>
       <c r="C302" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="303">
@@ -3702,7 +3702,7 @@
         <v>301</v>
       </c>
       <c r="C303" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="304">
@@ -3713,7 +3713,7 @@
         <v>302</v>
       </c>
       <c r="C304" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="305">
@@ -3724,7 +3724,7 @@
         <v>303</v>
       </c>
       <c r="C305" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="306">
@@ -3735,7 +3735,7 @@
         <v>304</v>
       </c>
       <c r="C306" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="307">
@@ -3746,7 +3746,7 @@
         <v>305</v>
       </c>
       <c r="C307" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="308">
@@ -3757,7 +3757,7 @@
         <v>306</v>
       </c>
       <c r="C308" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="309">
@@ -3768,7 +3768,7 @@
         <v>307</v>
       </c>
       <c r="C309" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="310">
@@ -3779,7 +3779,7 @@
         <v>308</v>
       </c>
       <c r="C310" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="311">
@@ -3790,7 +3790,7 @@
         <v>309</v>
       </c>
       <c r="C311" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="312">
@@ -3801,7 +3801,7 @@
         <v>310</v>
       </c>
       <c r="C312" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="313">
@@ -3812,7 +3812,7 @@
         <v>311</v>
       </c>
       <c r="C313" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="314">
@@ -3823,7 +3823,7 @@
         <v>312</v>
       </c>
       <c r="C314" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="315">
@@ -3834,7 +3834,7 @@
         <v>313</v>
       </c>
       <c r="C315" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="316">
@@ -3845,7 +3845,7 @@
         <v>314</v>
       </c>
       <c r="C316" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="317">
@@ -3856,7 +3856,7 @@
         <v>315</v>
       </c>
       <c r="C317" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="318">
@@ -3867,7 +3867,7 @@
         <v>316</v>
       </c>
       <c r="C318" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="319">
@@ -3878,7 +3878,7 @@
         <v>317</v>
       </c>
       <c r="C319" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="320">
@@ -3889,7 +3889,7 @@
         <v>318</v>
       </c>
       <c r="C320" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="321">
@@ -3900,7 +3900,7 @@
         <v>319</v>
       </c>
       <c r="C321" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="322">
@@ -3911,7 +3911,7 @@
         <v>320</v>
       </c>
       <c r="C322" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="323">
@@ -3922,7 +3922,7 @@
         <v>321</v>
       </c>
       <c r="C323" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="324">
@@ -3933,7 +3933,7 @@
         <v>322</v>
       </c>
       <c r="C324" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="325">
@@ -3944,7 +3944,7 @@
         <v>323</v>
       </c>
       <c r="C325" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="326">
@@ -3955,7 +3955,7 @@
         <v>324</v>
       </c>
       <c r="C326" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="327">
@@ -3966,7 +3966,7 @@
         <v>325</v>
       </c>
       <c r="C327" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="328">
@@ -3977,7 +3977,7 @@
         <v>326</v>
       </c>
       <c r="C328" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="329">
@@ -3988,7 +3988,7 @@
         <v>327</v>
       </c>
       <c r="C329" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="330">
@@ -3999,7 +3999,7 @@
         <v>328</v>
       </c>
       <c r="C330" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="331">
@@ -4010,7 +4010,7 @@
         <v>329</v>
       </c>
       <c r="C331" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="332">
@@ -4021,7 +4021,7 @@
         <v>330</v>
       </c>
       <c r="C332" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="333">
@@ -4032,7 +4032,7 @@
         <v>331</v>
       </c>
       <c r="C333" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="334">
@@ -4043,7 +4043,7 @@
         <v>332</v>
       </c>
       <c r="C334" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="335">
@@ -4054,7 +4054,7 @@
         <v>333</v>
       </c>
       <c r="C335" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="336">
@@ -4065,7 +4065,7 @@
         <v>334</v>
       </c>
       <c r="C336" t="n">
-        <v>7293</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="337">
@@ -4076,7 +4076,7 @@
         <v>335</v>
       </c>
       <c r="C337" t="n">
-        <v>7293</v>
+        <v>7295</v>
       </c>
     </row>
     <row r="338">
@@ -4087,7 +4087,7 @@
         <v>336</v>
       </c>
       <c r="C338" t="n">
-        <v>7293</v>
+        <v>7295</v>
       </c>
     </row>
     <row r="339">
@@ -4098,7 +4098,7 @@
         <v>337</v>
       </c>
       <c r="C339" t="n">
-        <v>7293</v>
+        <v>7295</v>
       </c>
     </row>
     <row r="340">
@@ -4109,7 +4109,7 @@
         <v>338</v>
       </c>
       <c r="C340" t="n">
-        <v>7293</v>
+        <v>7295</v>
       </c>
     </row>
     <row r="341">
@@ -4120,7 +4120,7 @@
         <v>339</v>
       </c>
       <c r="C341" t="n">
-        <v>7293</v>
+        <v>7295</v>
       </c>
     </row>
     <row r="342">
@@ -4131,7 +4131,7 @@
         <v>340</v>
       </c>
       <c r="C342" t="n">
-        <v>7293</v>
+        <v>7295</v>
       </c>
     </row>
     <row r="343">
@@ -4142,7 +4142,7 @@
         <v>341</v>
       </c>
       <c r="C343" t="n">
-        <v>7293</v>
+        <v>7295</v>
       </c>
     </row>
     <row r="344">
@@ -4153,7 +4153,7 @@
         <v>342</v>
       </c>
       <c r="C344" t="n">
-        <v>7293</v>
+        <v>7295</v>
       </c>
     </row>
     <row r="345">
@@ -4164,7 +4164,7 @@
         <v>343</v>
       </c>
       <c r="C345" t="n">
-        <v>7293</v>
+        <v>7295</v>
       </c>
     </row>
     <row r="346">
@@ -4175,7 +4175,7 @@
         <v>344</v>
       </c>
       <c r="C346" t="n">
-        <v>7293</v>
+        <v>7295</v>
       </c>
     </row>
     <row r="347">
@@ -4186,7 +4186,7 @@
         <v>345</v>
       </c>
       <c r="C347" t="n">
-        <v>7293</v>
+        <v>7295</v>
       </c>
     </row>
     <row r="348">
@@ -4197,7 +4197,7 @@
         <v>346</v>
       </c>
       <c r="C348" t="n">
-        <v>7293</v>
+        <v>7295</v>
       </c>
     </row>
     <row r="349">
@@ -4208,7 +4208,7 @@
         <v>347</v>
       </c>
       <c r="C349" t="n">
-        <v>7293</v>
+        <v>7295</v>
       </c>
     </row>
     <row r="350">
@@ -4219,7 +4219,7 @@
         <v>348</v>
       </c>
       <c r="C350" t="n">
-        <v>7293</v>
+        <v>7295</v>
       </c>
     </row>
     <row r="351">
@@ -4230,7 +4230,7 @@
         <v>349</v>
       </c>
       <c r="C351" t="n">
-        <v>7293</v>
+        <v>7295</v>
       </c>
     </row>
     <row r="352">
@@ -4241,7 +4241,7 @@
         <v>350</v>
       </c>
       <c r="C352" t="n">
-        <v>7293</v>
+        <v>7295</v>
       </c>
     </row>
     <row r="353">
@@ -4252,7 +4252,7 @@
         <v>351</v>
       </c>
       <c r="C353" t="n">
-        <v>7293</v>
+        <v>7295</v>
       </c>
     </row>
     <row r="354">
@@ -4263,7 +4263,7 @@
         <v>352</v>
       </c>
       <c r="C354" t="n">
-        <v>7293</v>
+        <v>7295</v>
       </c>
     </row>
     <row r="355">
@@ -4274,7 +4274,7 @@
         <v>353</v>
       </c>
       <c r="C355" t="n">
-        <v>7293</v>
+        <v>7295</v>
       </c>
     </row>
     <row r="356">
@@ -4285,7 +4285,7 @@
         <v>354</v>
       </c>
       <c r="C356" t="n">
-        <v>7293</v>
+        <v>7295</v>
       </c>
     </row>
     <row r="357">
@@ -4296,7 +4296,7 @@
         <v>355</v>
       </c>
       <c r="C357" t="n">
-        <v>7293</v>
+        <v>7295</v>
       </c>
     </row>
     <row r="358">
@@ -4307,7 +4307,7 @@
         <v>356</v>
       </c>
       <c r="C358" t="n">
-        <v>7293</v>
+        <v>7295</v>
       </c>
     </row>
     <row r="359">
@@ -4318,7 +4318,7 @@
         <v>357</v>
       </c>
       <c r="C359" t="n">
-        <v>7293</v>
+        <v>7295</v>
       </c>
     </row>
     <row r="360">
@@ -4329,7 +4329,7 @@
         <v>358</v>
       </c>
       <c r="C360" t="n">
-        <v>7293</v>
+        <v>7295</v>
       </c>
     </row>
     <row r="361">
@@ -4340,7 +4340,7 @@
         <v>359</v>
       </c>
       <c r="C361" t="n">
-        <v>7293</v>
+        <v>7295</v>
       </c>
     </row>
     <row r="362">
@@ -4351,7 +4351,7 @@
         <v>360</v>
       </c>
       <c r="C362" t="n">
-        <v>7293</v>
+        <v>7295</v>
       </c>
     </row>
     <row r="363">
@@ -4362,7 +4362,7 @@
         <v>361</v>
       </c>
       <c r="C363" t="n">
-        <v>7293</v>
+        <v>7295</v>
       </c>
     </row>
     <row r="364">
@@ -4373,7 +4373,7 @@
         <v>362</v>
       </c>
       <c r="C364" t="n">
-        <v>7293</v>
+        <v>7295</v>
       </c>
     </row>
     <row r="365">
@@ -4384,7 +4384,7 @@
         <v>363</v>
       </c>
       <c r="C365" t="n">
-        <v>7293</v>
+        <v>7295</v>
       </c>
     </row>
     <row r="366">
@@ -4395,7 +4395,7 @@
         <v>364</v>
       </c>
       <c r="C366" t="n">
-        <v>7293</v>
+        <v>7295</v>
       </c>
     </row>
     <row r="367">
@@ -4406,7 +4406,7 @@
         <v>365</v>
       </c>
       <c r="C367" t="n">
-        <v>7293</v>
+        <v>7295</v>
       </c>
     </row>
     <row r="368">
@@ -4417,7 +4417,7 @@
         <v>366</v>
       </c>
       <c r="C368" t="n">
-        <v>7293</v>
+        <v>7295</v>
       </c>
     </row>
     <row r="369">
@@ -4428,7 +4428,7 @@
         <v>367</v>
       </c>
       <c r="C369" t="n">
-        <v>7293</v>
+        <v>7295</v>
       </c>
     </row>
     <row r="370">
@@ -4439,7 +4439,7 @@
         <v>368</v>
       </c>
       <c r="C370" t="n">
-        <v>7293</v>
+        <v>7295</v>
       </c>
     </row>
     <row r="371">
@@ -4450,7 +4450,7 @@
         <v>369</v>
       </c>
       <c r="C371" t="n">
-        <v>7293</v>
+        <v>7295</v>
       </c>
     </row>
     <row r="372">
@@ -4461,7 +4461,7 @@
         <v>370</v>
       </c>
       <c r="C372" t="n">
-        <v>7293</v>
+        <v>7295</v>
       </c>
     </row>
     <row r="373">
@@ -4472,7 +4472,7 @@
         <v>371</v>
       </c>
       <c r="C373" t="n">
-        <v>7293</v>
+        <v>7295</v>
       </c>
     </row>
     <row r="374">
@@ -4483,7 +4483,7 @@
         <v>372</v>
       </c>
       <c r="C374" t="n">
-        <v>7293</v>
+        <v>7295</v>
       </c>
     </row>
     <row r="375">
@@ -4494,7 +4494,7 @@
         <v>373</v>
       </c>
       <c r="C375" t="n">
-        <v>7293</v>
+        <v>7295</v>
       </c>
     </row>
     <row r="376">
@@ -4505,7 +4505,7 @@
         <v>374</v>
       </c>
       <c r="C376" t="n">
-        <v>7293</v>
+        <v>7295</v>
       </c>
     </row>
     <row r="377">
@@ -4516,7 +4516,7 @@
         <v>375</v>
       </c>
       <c r="C377" t="n">
-        <v>7293</v>
+        <v>7295</v>
       </c>
     </row>
     <row r="378">

</xml_diff>